<commit_message>
Updated Sed and Ruppia import
</commit_message>
<xml_diff>
--- a/data/incoming/TandI_1/Sediment/UNI012-SS-K5799 Sediment Results Feb-Mar 2021 Leslie_Luke.xlsx
+++ b/data/incoming/TandI_1/Sediment/UNI012-SS-K5799 Sediment Results Feb-Mar 2021 Leslie_Luke.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr date1904="1" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1675510\Box\Coorong Project - Team share folder\DEW Share Files and Photos\Sediment Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\data\incoming\TandI_1\Sediment\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAD8AD3-ECBC-4392-953B-FAA8BFF037EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13200"/>
+    <workbookView xWindow="20" yWindow="10" windowWidth="25580" windowHeight="15380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SitesMetaData" sheetId="18" r:id="rId1"/>
     <sheet name="Data" sheetId="17" r:id="rId2"/>
     <sheet name="Data2" sheetId="19" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -601,9 +613,6 @@
     <t xml:space="preserve">1M HCL Extract - APHA 3125 ICPMS </t>
   </si>
   <si>
-    <t>Parrnka A 0-3 cm</t>
-  </si>
-  <si>
     <t>K5798/1</t>
   </si>
   <si>
@@ -704,9 +713,6 @@
   </si>
   <si>
     <t>K5798/16</t>
-  </si>
-  <si>
-    <t>Villa de Yumpa</t>
   </si>
   <si>
     <t>K5798/17</t>
@@ -765,16 +771,22 @@
   <si>
     <t>HideRow</t>
   </si>
+  <si>
+    <t>Parrnka A 0-3cm</t>
+  </si>
+  <si>
+    <t>Villa de Yumpa 0-3cm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000"/>
-    <numFmt numFmtId="171" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1263,6 +1275,58 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -1287,69 +1351,17 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1452,7 +1464,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1507,7 +1519,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1889,24 +1901,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="29.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" ht="13.5" thickBot="1">
+    <row r="3" spans="1:6" ht="13" thickBot="1">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -1951,7 +1963,7 @@
         <v>139.2621833</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="39" thickBot="1">
+    <row r="6" spans="1:6" ht="39.5" thickBot="1">
       <c r="A6" s="40" t="s">
         <v>87</v>
       </c>
@@ -1971,7 +1983,7 @@
         <v>139.39676</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="26.25" thickBot="1">
+    <row r="7" spans="1:6" ht="26.5" thickBot="1">
       <c r="A7" s="40" t="s">
         <v>90</v>
       </c>
@@ -1991,7 +2003,7 @@
         <v>139.58403000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="39" thickBot="1">
+    <row r="8" spans="1:6" ht="39.5" thickBot="1">
       <c r="A8" s="40" t="s">
         <v>87</v>
       </c>
@@ -2011,7 +2023,7 @@
         <v>139.39743200000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="64.5" thickBot="1">
+    <row r="9" spans="1:6" ht="65.5" thickBot="1">
       <c r="A9" s="40" t="s">
         <v>90</v>
       </c>
@@ -2031,7 +2043,7 @@
         <v>139.58401720000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="26.25" thickBot="1">
+    <row r="10" spans="1:6" ht="13.5" thickBot="1">
       <c r="A10" s="40" t="s">
         <v>95</v>
       </c>
@@ -2051,35 +2063,35 @@
         <v>139.6114</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="47" t="s">
+    <row r="11" spans="1:6" ht="13">
+      <c r="A11" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="67">
         <v>42766</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="69" t="s">
         <v>100</v>
       </c>
       <c r="E11" s="45">
         <v>-35.951599999999999</v>
       </c>
-      <c r="F11" s="53">
+      <c r="F11" s="71">
         <v>139.49170000000001</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.5" thickBot="1">
-      <c r="A12" s="48"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="52"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="F12" s="54"/>
+      <c r="F12" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2094,25 +2106,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="21" customWidth="1"/>
-    <col min="3" max="7" width="15.7109375" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="24.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="21" customWidth="1"/>
+    <col min="3" max="7" width="15.7265625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="11.453125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25">
+    <row r="1" spans="1:7" ht="23">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -2155,7 +2167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26.25" thickBot="1">
+    <row r="6" spans="1:7" ht="13.5" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>1</v>
       </c>
@@ -2208,7 +2220,7 @@
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
     </row>
-    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>27</v>
       </c>
@@ -2231,7 +2243,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>28</v>
       </c>
@@ -2254,7 +2266,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>29</v>
       </c>
@@ -2277,7 +2289,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>30</v>
       </c>
@@ -2300,7 +2312,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>31</v>
       </c>
@@ -2323,7 +2335,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>32</v>
       </c>
@@ -2346,7 +2358,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>33</v>
       </c>
@@ -2369,7 +2381,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>34</v>
       </c>
@@ -2392,7 +2404,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>35</v>
       </c>
@@ -2415,7 +2427,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>36</v>
       </c>
@@ -2438,7 +2450,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>37</v>
       </c>
@@ -2461,7 +2473,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>38</v>
       </c>
@@ -2484,7 +2496,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A21" s="16" t="s">
         <v>39</v>
       </c>
@@ -2507,7 +2519,7 @@
         <v>5.56</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A22" s="16" t="s">
         <v>40</v>
       </c>
@@ -2530,7 +2542,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A23" s="16" t="s">
         <v>41</v>
       </c>
@@ -2553,7 +2565,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A24" s="16" t="s">
         <v>42</v>
       </c>
@@ -2576,7 +2588,7 @@
         <v>7.98</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="25" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A25" s="16" t="s">
         <v>43</v>
       </c>
@@ -2599,7 +2611,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="26" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A26" s="16" t="s">
         <v>44</v>
       </c>
@@ -2622,7 +2634,7 @@
         <v>7.29</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="27" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A27" s="16" t="s">
         <v>45</v>
       </c>
@@ -2645,7 +2657,7 @@
         <v>7.69</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="20.100000000000001" customHeight="1">
+    <row r="28" spans="1:10" ht="20.149999999999999" customHeight="1">
       <c r="A28" s="16" t="s">
         <v>46</v>
       </c>
@@ -2668,7 +2680,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15">
+    <row r="29" spans="1:10" ht="15.5">
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
       <c r="C29" s="26"/>
@@ -2677,7 +2689,7 @@
       <c r="F29" s="26"/>
       <c r="G29" s="26"/>
     </row>
-    <row r="30" spans="1:10" ht="6.95" customHeight="1">
+    <row r="30" spans="1:10" ht="7" customHeight="1">
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -2895,7 +2907,7 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.51" right="0.51" top="0.51" bottom="1.3737007874015748" header="0.39000000000000007" footer="0.39000000000000007"/>
-  <pageSetup paperSize="9" scale="64" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="62" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;12PAGE &amp;P OF &amp;N</oddHeader>
     <oddFooter>&amp;C&amp;12&amp;K008000Environmental Analysis Laboratory, Southern Cross University, 
@@ -2910,58 +2922,58 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="21" customWidth="1"/>
-    <col min="3" max="23" width="14.7109375" style="55" customWidth="1"/>
-    <col min="24" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="24.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" style="21" customWidth="1"/>
+    <col min="3" max="23" width="14.7265625" style="47" customWidth="1"/>
+    <col min="24" max="16384" width="11.453125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="23.25">
+    <row r="1" spans="1:23" ht="23">
       <c r="A1" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:23" ht="15.75">
+    <row r="2" spans="1:23" ht="15.5">
       <c r="A2" s="4" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-    </row>
-    <row r="3" spans="1:23" ht="14.1" customHeight="1">
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+    </row>
+    <row r="3" spans="1:23" ht="14.15" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>48</v>
       </c>
@@ -2976,1486 +2988,1486 @@
     <row r="5" spans="1:23" ht="42.75" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59" t="s">
+      <c r="D5" s="74"/>
+      <c r="E5" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="M5" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="N5" s="59" t="s">
+      <c r="N5" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="P5" s="59" t="s">
+      <c r="P5" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="Q5" s="59" t="s">
+      <c r="Q5" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="R5" s="59" t="s">
+      <c r="R5" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="S5" s="59" t="s">
+      <c r="S5" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="T5" s="59" t="s">
+      <c r="T5" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="U5" s="59" t="s">
+      <c r="U5" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="V5" s="59" t="s">
+      <c r="V5" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="W5" s="59" t="s">
+      <c r="W5" s="49" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="22" customFormat="1" ht="36.950000000000003" customHeight="1" thickBot="1">
-      <c r="A6" s="60" t="s">
+    <row r="6" spans="1:23" s="22" customFormat="1" ht="37" customHeight="1" thickBot="1">
+      <c r="A6" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="62" t="s">
+      <c r="E6" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="62" t="s">
+      <c r="F6" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="62" t="s">
+      <c r="G6" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="H6" s="62" t="s">
+      <c r="H6" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="I6" s="62" t="s">
+      <c r="I6" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="62" t="s">
+      <c r="J6" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="K6" s="62" t="s">
+      <c r="K6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="L6" s="62" t="s">
+      <c r="L6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="M6" s="62" t="s">
+      <c r="M6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="N6" s="62" t="s">
+      <c r="N6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="O6" s="62" t="s">
+      <c r="O6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="P6" s="62" t="s">
+      <c r="P6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="Q6" s="62" t="s">
+      <c r="Q6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="R6" s="62" t="s">
+      <c r="R6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="S6" s="62" t="s">
+      <c r="S6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="T6" s="62" t="s">
+      <c r="T6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="U6" s="62" t="s">
+      <c r="U6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="V6" s="62" t="s">
+      <c r="V6" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="W6" s="62" t="s">
+      <c r="W6" s="52" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="33.950000000000003" customHeight="1" thickTop="1">
+    <row r="7" spans="1:23" ht="34" customHeight="1" thickTop="1">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="63" t="s">
+      <c r="F7" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="63" t="s">
+      <c r="G7" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="63" t="s">
+      <c r="H7" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="I7" s="63" t="s">
+      <c r="I7" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="63" t="s">
+      <c r="J7" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="64" t="s">
+      <c r="K7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="L7" s="64" t="s">
+      <c r="L7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="M7" s="64" t="s">
+      <c r="M7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="N7" s="64" t="s">
+      <c r="N7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="O7" s="64" t="s">
+      <c r="O7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P7" s="64" t="s">
+      <c r="P7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="Q7" s="64" t="s">
+      <c r="Q7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="R7" s="64" t="s">
+      <c r="R7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="S7" s="64" t="s">
+      <c r="S7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="T7" s="64" t="s">
+      <c r="T7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="U7" s="64" t="s">
+      <c r="U7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="V7" s="64" t="s">
+      <c r="V7" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="W7" s="64" t="s">
+      <c r="W7" s="54" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15">
+    <row r="8" spans="1:23" ht="15.5">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65"/>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="65"/>
-      <c r="S8" s="65"/>
-      <c r="T8" s="65"/>
-      <c r="U8" s="65"/>
-      <c r="V8" s="65"/>
-      <c r="W8" s="65"/>
-    </row>
-    <row r="9" spans="1:23" ht="20.100000000000001" customHeight="1">
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
+      <c r="V8" s="55"/>
+      <c r="W8" s="55"/>
+    </row>
+    <row r="9" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A9" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="66">
+      <c r="C9" s="56">
         <v>9.0888016927064094E-2</v>
       </c>
-      <c r="D9" s="67">
+      <c r="D9" s="57">
         <f>C9*623.7</f>
         <v>56.686856157409878</v>
       </c>
-      <c r="E9" s="66">
+      <c r="E9" s="56">
         <v>8.76</v>
       </c>
-      <c r="F9" s="66">
+      <c r="F9" s="56">
         <v>10.834149999999999</v>
       </c>
-      <c r="G9" s="67">
+      <c r="G9" s="57">
         <v>228</v>
       </c>
-      <c r="H9" s="68">
+      <c r="H9" s="58">
         <v>1.8083182640144663E-3</v>
       </c>
-      <c r="I9" s="66">
+      <c r="I9" s="56">
         <v>0.66600000000000004</v>
       </c>
-      <c r="J9" s="66">
+      <c r="J9" s="56">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="K9" s="66" t="s">
+      <c r="K9" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L9" s="59">
+        <v>2.1073582315994499</v>
+      </c>
+      <c r="M9" s="59">
+        <v>1.2775810941399299</v>
+      </c>
+      <c r="N9" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L9" s="69">
-        <v>2.1073582315994499</v>
-      </c>
-      <c r="M9" s="69">
-        <v>1.2775810941399299</v>
-      </c>
-      <c r="N9" s="66" t="s">
+      <c r="O9" s="59">
+        <v>1.2515548788814499</v>
+      </c>
+      <c r="P9" s="59">
+        <v>0.93770927667857396</v>
+      </c>
+      <c r="Q9" s="57">
+        <v>38.345805552445299</v>
+      </c>
+      <c r="R9" s="59">
+        <v>0.54042676037583603</v>
+      </c>
+      <c r="S9" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="T9" s="59">
+        <v>2.5612860508124098</v>
+      </c>
+      <c r="U9" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O9" s="69">
-        <v>1.2515548788814499</v>
-      </c>
-      <c r="P9" s="69">
-        <v>0.93770927667857396</v>
-      </c>
-      <c r="Q9" s="67">
-        <v>38.345805552445299</v>
-      </c>
-      <c r="R9" s="69">
-        <v>0.54042676037583603</v>
-      </c>
-      <c r="S9" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="T9" s="69">
-        <v>2.5612860508124098</v>
-      </c>
-      <c r="U9" s="66" t="s">
+      <c r="V9" s="57">
+        <v>651.56022203834402</v>
+      </c>
+      <c r="W9" s="57">
+        <v>388.48800538156797</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="20.149999999999999" customHeight="1">
+      <c r="A10" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="V9" s="67">
-        <v>651.56022203834402</v>
-      </c>
-      <c r="W9" s="67">
-        <v>388.48800538156797</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C10" s="66">
+      <c r="C10" s="56">
         <v>0.12163413706081386</v>
       </c>
-      <c r="D10" s="67">
+      <c r="D10" s="57">
         <f t="shared" ref="D10:D25" si="0">C10*623.7</f>
         <v>75.863211284829603</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="56">
         <v>8.9499999999999993</v>
       </c>
-      <c r="F10" s="66">
+      <c r="F10" s="56">
         <v>10.06892</v>
       </c>
-      <c r="G10" s="67">
+      <c r="G10" s="57">
         <v>154</v>
       </c>
-      <c r="H10" s="68">
+      <c r="H10" s="58">
         <v>4.6965903882091571E-3</v>
       </c>
-      <c r="I10" s="66">
+      <c r="I10" s="56">
         <v>0.69499999999999995</v>
       </c>
-      <c r="J10" s="66">
+      <c r="J10" s="56">
         <v>0.06</v>
       </c>
-      <c r="K10" s="66" t="s">
+      <c r="K10" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L10" s="59">
+        <v>1.10429448950885</v>
+      </c>
+      <c r="M10" s="59">
+        <v>1.38452406803081</v>
+      </c>
+      <c r="N10" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L10" s="69">
-        <v>1.10429448950885</v>
-      </c>
-      <c r="M10" s="69">
-        <v>1.38452406803081</v>
-      </c>
-      <c r="N10" s="66" t="s">
+      <c r="O10" s="59">
+        <v>1.6995844542360901</v>
+      </c>
+      <c r="P10" s="59">
+        <v>1.06629721271845</v>
+      </c>
+      <c r="Q10" s="57">
+        <v>46.184048557559301</v>
+      </c>
+      <c r="R10" s="59">
+        <v>0.61270532594702898</v>
+      </c>
+      <c r="S10" s="59">
+        <v>0.71007322115271099</v>
+      </c>
+      <c r="T10" s="59">
+        <v>2.24500289454086</v>
+      </c>
+      <c r="U10" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O10" s="69">
-        <v>1.6995844542360901</v>
-      </c>
-      <c r="P10" s="69">
-        <v>1.06629721271845</v>
-      </c>
-      <c r="Q10" s="67">
-        <v>46.184048557559301</v>
-      </c>
-      <c r="R10" s="69">
-        <v>0.61270532594702898</v>
-      </c>
-      <c r="S10" s="69">
-        <v>0.71007322115271099</v>
-      </c>
-      <c r="T10" s="69">
-        <v>2.24500289454086</v>
-      </c>
-      <c r="U10" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V10" s="67">
+      <c r="V10" s="57">
         <v>856.92303872641696</v>
       </c>
-      <c r="W10" s="67">
+      <c r="W10" s="57">
         <v>617.90541480867603</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A11" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" s="66">
+      <c r="C11" s="56">
         <v>0.16003424345101497</v>
       </c>
-      <c r="D11" s="67">
+      <c r="D11" s="57">
         <f t="shared" si="0"/>
         <v>99.813357640398038</v>
       </c>
-      <c r="E11" s="66">
+      <c r="E11" s="56">
         <v>9.0299999999999994</v>
       </c>
-      <c r="F11" s="66">
+      <c r="F11" s="56">
         <v>12.28612</v>
       </c>
-      <c r="G11" s="67">
+      <c r="G11" s="57">
         <v>131</v>
       </c>
-      <c r="H11" s="68">
+      <c r="H11" s="58">
         <v>4.9716553996359538E-3</v>
       </c>
-      <c r="I11" s="66">
+      <c r="I11" s="56">
         <v>0.90500000000000003</v>
       </c>
-      <c r="J11" s="66">
+      <c r="J11" s="56">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K11" s="66" t="s">
+      <c r="K11" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L11" s="59">
+        <v>1.0688983750630701</v>
+      </c>
+      <c r="M11" s="59">
+        <v>1.6963798576315601</v>
+      </c>
+      <c r="N11" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L11" s="69">
-        <v>1.0688983750630701</v>
-      </c>
-      <c r="M11" s="69">
-        <v>1.6963798576315601</v>
-      </c>
-      <c r="N11" s="66" t="s">
+      <c r="O11" s="59">
+        <v>1.7898015220424399</v>
+      </c>
+      <c r="P11" s="59">
+        <v>1.4620475197677101</v>
+      </c>
+      <c r="Q11" s="57">
+        <v>42.794082187255398</v>
+      </c>
+      <c r="R11" s="59">
+        <v>0.87660564230765803</v>
+      </c>
+      <c r="S11" s="59">
+        <v>0.48968469692882099</v>
+      </c>
+      <c r="T11" s="59">
+        <v>2.7076682799454801</v>
+      </c>
+      <c r="U11" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O11" s="69">
-        <v>1.7898015220424399</v>
-      </c>
-      <c r="P11" s="69">
-        <v>1.4620475197677101</v>
-      </c>
-      <c r="Q11" s="67">
-        <v>42.794082187255398</v>
-      </c>
-      <c r="R11" s="69">
-        <v>0.87660564230765803</v>
-      </c>
-      <c r="S11" s="69">
-        <v>0.48968469692882099</v>
-      </c>
-      <c r="T11" s="69">
-        <v>2.7076682799454801</v>
-      </c>
-      <c r="U11" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V11" s="67">
+      <c r="V11" s="57">
         <v>969.69870932374101</v>
       </c>
-      <c r="W11" s="67">
+      <c r="W11" s="57">
         <v>791.12258816261897</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A12" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="66">
+      <c r="C12" s="56">
         <v>8.2951592858909351E-2</v>
       </c>
-      <c r="D12" s="67">
+      <c r="D12" s="57">
         <f t="shared" si="0"/>
         <v>51.736908466101767</v>
       </c>
-      <c r="E12" s="66">
+      <c r="E12" s="56">
         <v>9.14</v>
       </c>
-      <c r="F12" s="66">
+      <c r="F12" s="56">
         <v>9.5783899999999988</v>
       </c>
-      <c r="G12" s="67">
+      <c r="G12" s="57">
         <v>106</v>
       </c>
-      <c r="H12" s="68">
+      <c r="H12" s="58">
         <v>4.7700972628908437E-3</v>
       </c>
-      <c r="I12" s="66">
+      <c r="I12" s="56">
         <v>0.55699999999999994</v>
       </c>
-      <c r="J12" s="66">
+      <c r="J12" s="56">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="K12" s="66" t="s">
+      <c r="K12" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L12" s="59">
+        <v>1.5452700407097699</v>
+      </c>
+      <c r="M12" s="59">
+        <v>1.10387479324325</v>
+      </c>
+      <c r="N12" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L12" s="69">
-        <v>1.5452700407097699</v>
-      </c>
-      <c r="M12" s="69">
-        <v>1.10387479324325</v>
-      </c>
-      <c r="N12" s="66" t="s">
+      <c r="O12" s="59">
+        <v>1.45328051622726</v>
+      </c>
+      <c r="P12" s="59">
+        <v>0.92066869971913201</v>
+      </c>
+      <c r="Q12" s="57">
+        <v>39.971397160340501</v>
+      </c>
+      <c r="R12" s="59">
+        <v>0.55271042180598096</v>
+      </c>
+      <c r="S12" s="59">
+        <v>0.371050338154369</v>
+      </c>
+      <c r="T12" s="59">
+        <v>1.55995745621841</v>
+      </c>
+      <c r="U12" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O12" s="69">
-        <v>1.45328051622726</v>
-      </c>
-      <c r="P12" s="69">
-        <v>0.92066869971913201</v>
-      </c>
-      <c r="Q12" s="67">
-        <v>39.971397160340501</v>
-      </c>
-      <c r="R12" s="69">
-        <v>0.55271042180598096</v>
-      </c>
-      <c r="S12" s="69">
-        <v>0.371050338154369</v>
-      </c>
-      <c r="T12" s="69">
-        <v>1.55995745621841</v>
-      </c>
-      <c r="U12" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V12" s="67">
+      <c r="V12" s="57">
         <v>609.28477326594998</v>
       </c>
-      <c r="W12" s="67">
+      <c r="W12" s="57">
         <v>443.78859589141098</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A13" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="66">
+      <c r="C13" s="56">
         <v>7.210099759443879E-2</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="57">
         <f t="shared" si="0"/>
         <v>44.969392199651473</v>
       </c>
-      <c r="E13" s="66">
+      <c r="E13" s="56">
         <v>9.1199999999999992</v>
       </c>
-      <c r="F13" s="66">
+      <c r="F13" s="56">
         <v>10.137600000000001</v>
       </c>
-      <c r="G13" s="67">
+      <c r="G13" s="57">
         <v>142</v>
       </c>
-      <c r="H13" s="68">
+      <c r="H13" s="58">
         <v>7.2713311315617266E-3</v>
       </c>
-      <c r="I13" s="66">
+      <c r="I13" s="56">
         <v>0.71299999999999997</v>
       </c>
-      <c r="J13" s="66">
+      <c r="J13" s="56">
         <v>5.45E-2</v>
       </c>
-      <c r="K13" s="66" t="s">
+      <c r="K13" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L13" s="59">
+        <v>2.2769533440983301</v>
+      </c>
+      <c r="M13" s="59">
+        <v>1.2053071363332499</v>
+      </c>
+      <c r="N13" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L13" s="69">
-        <v>2.2769533440983301</v>
-      </c>
-      <c r="M13" s="69">
-        <v>1.2053071363332499</v>
-      </c>
-      <c r="N13" s="66" t="s">
+      <c r="O13" s="59">
+        <v>1.36727271304084</v>
+      </c>
+      <c r="P13" s="59">
+        <v>1.0936609778269499</v>
+      </c>
+      <c r="Q13" s="57">
+        <v>38.461325493359702</v>
+      </c>
+      <c r="R13" s="59">
+        <v>0.463882063032661</v>
+      </c>
+      <c r="S13" s="59">
+        <v>0.147813265223321</v>
+      </c>
+      <c r="T13" s="59">
+        <v>2.1959705511680099</v>
+      </c>
+      <c r="U13" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O13" s="69">
-        <v>1.36727271304084</v>
-      </c>
-      <c r="P13" s="69">
-        <v>1.0936609778269499</v>
-      </c>
-      <c r="Q13" s="67">
-        <v>38.461325493359702</v>
-      </c>
-      <c r="R13" s="69">
-        <v>0.463882063032661</v>
-      </c>
-      <c r="S13" s="69">
-        <v>0.147813265223321</v>
-      </c>
-      <c r="T13" s="69">
-        <v>2.1959705511680099</v>
-      </c>
-      <c r="U13" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V13" s="67">
+      <c r="V13" s="57">
         <v>636.66004015713997</v>
       </c>
-      <c r="W13" s="67">
+      <c r="W13" s="57">
         <v>405.97465627023598</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A14" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="66">
+      <c r="C14" s="56">
         <v>0.18190572762883001</v>
       </c>
-      <c r="D14" s="67">
+      <c r="D14" s="57">
         <f t="shared" si="0"/>
         <v>113.45460232210128</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="56">
         <v>8.93</v>
       </c>
-      <c r="F14" s="66">
+      <c r="F14" s="56">
         <v>11.412979999999999</v>
       </c>
-      <c r="G14" s="67">
+      <c r="G14" s="57">
         <v>133</v>
       </c>
-      <c r="H14" s="68">
+      <c r="H14" s="58">
         <v>4.6264765975435052E-3</v>
       </c>
-      <c r="I14" s="66">
+      <c r="I14" s="56">
         <v>1.23</v>
       </c>
-      <c r="J14" s="66">
+      <c r="J14" s="56">
         <v>0.105</v>
       </c>
-      <c r="K14" s="66" t="s">
+      <c r="K14" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L14" s="59">
+        <v>1.4750843373946401</v>
+      </c>
+      <c r="M14" s="59">
+        <v>2.25696388228112</v>
+      </c>
+      <c r="N14" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L14" s="69">
-        <v>1.4750843373946401</v>
-      </c>
-      <c r="M14" s="69">
-        <v>2.25696388228112</v>
-      </c>
-      <c r="N14" s="66" t="s">
+      <c r="O14" s="59">
+        <v>2.1243373762412201</v>
+      </c>
+      <c r="P14" s="59">
+        <v>2.1551806614341502</v>
+      </c>
+      <c r="Q14" s="57">
+        <v>48.210506545132901</v>
+      </c>
+      <c r="R14" s="59">
+        <v>1.1774457632059101</v>
+      </c>
+      <c r="S14" s="59">
+        <v>5.9373490512371098E-2</v>
+      </c>
+      <c r="T14" s="59">
+        <v>3.3071805644466199</v>
+      </c>
+      <c r="U14" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O14" s="69">
-        <v>2.1243373762412201</v>
-      </c>
-      <c r="P14" s="69">
-        <v>2.1551806614341502</v>
-      </c>
-      <c r="Q14" s="67">
-        <v>48.210506545132901</v>
-      </c>
-      <c r="R14" s="69">
-        <v>1.1774457632059101</v>
-      </c>
-      <c r="S14" s="69">
-        <v>5.9373490512371098E-2</v>
-      </c>
-      <c r="T14" s="69">
-        <v>3.3071805644466199</v>
-      </c>
-      <c r="U14" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V14" s="67">
+      <c r="V14" s="57">
         <v>1282.07420527217</v>
       </c>
-      <c r="W14" s="67">
+      <c r="W14" s="57">
         <v>1079.4301766947101</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A15" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="66">
+      <c r="C15" s="56">
         <v>0.16390493286617805</v>
       </c>
-      <c r="D15" s="67">
+      <c r="D15" s="57">
         <f t="shared" si="0"/>
         <v>102.22750662863525</v>
       </c>
-      <c r="E15" s="66">
+      <c r="E15" s="56">
         <v>8.9499999999999993</v>
       </c>
-      <c r="F15" s="66">
+      <c r="F15" s="56">
         <v>16.74015</v>
       </c>
-      <c r="G15" s="67">
+      <c r="G15" s="57">
         <v>159</v>
       </c>
-      <c r="H15" s="68">
+      <c r="H15" s="58">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I15" s="66">
+      <c r="I15" s="56">
         <v>1.44</v>
       </c>
-      <c r="J15" s="66">
+      <c r="J15" s="56">
         <v>0.13900000000000001</v>
       </c>
-      <c r="K15" s="66" t="s">
+      <c r="K15" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L15" s="59">
+        <v>3.5760332751059298</v>
+      </c>
+      <c r="M15" s="59">
+        <v>2.6292268388284201</v>
+      </c>
+      <c r="N15" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L15" s="69">
-        <v>3.5760332751059298</v>
-      </c>
-      <c r="M15" s="69">
-        <v>2.6292268388284201</v>
-      </c>
-      <c r="N15" s="66" t="s">
+      <c r="O15" s="59">
+        <v>2.1214158153973601</v>
+      </c>
+      <c r="P15" s="59">
+        <v>2.1522642320085699</v>
+      </c>
+      <c r="Q15" s="57">
+        <v>48.674706972594798</v>
+      </c>
+      <c r="R15" s="59">
+        <v>1.2283963264537601</v>
+      </c>
+      <c r="S15" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="T15" s="59">
+        <v>5.4451257497991596</v>
+      </c>
+      <c r="U15" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O15" s="69">
-        <v>2.1214158153973601</v>
-      </c>
-      <c r="P15" s="69">
-        <v>2.1522642320085699</v>
-      </c>
-      <c r="Q15" s="67">
-        <v>48.674706972594798</v>
-      </c>
-      <c r="R15" s="69">
-        <v>1.2283963264537601</v>
-      </c>
-      <c r="S15" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="T15" s="69">
-        <v>5.4451257497991596</v>
-      </c>
-      <c r="U15" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V15" s="67">
+      <c r="V15" s="57">
         <v>1334.8365088732101</v>
       </c>
-      <c r="W15" s="67">
+      <c r="W15" s="57">
         <v>1071.69627350664</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A16" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="66">
+      <c r="C16" s="56">
         <v>0.13755708635630201</v>
       </c>
-      <c r="D16" s="67">
+      <c r="D16" s="57">
         <f t="shared" si="0"/>
         <v>85.794354760425577</v>
       </c>
-      <c r="E16" s="66">
+      <c r="E16" s="56">
         <v>9.0399999999999991</v>
       </c>
-      <c r="F16" s="66">
+      <c r="F16" s="56">
         <v>12.29594</v>
       </c>
-      <c r="G16" s="67">
+      <c r="G16" s="57">
         <v>131</v>
       </c>
-      <c r="H16" s="68">
+      <c r="H16" s="58">
         <v>2.5591362915016167E-3</v>
       </c>
-      <c r="I16" s="66">
+      <c r="I16" s="56">
         <v>0.80400000000000005</v>
       </c>
-      <c r="J16" s="66">
+      <c r="J16" s="56">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="K16" s="66" t="s">
+      <c r="K16" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L16" s="59">
+        <v>1.3771867981000101</v>
+      </c>
+      <c r="M16" s="59">
+        <v>1.7106868645080799</v>
+      </c>
+      <c r="N16" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L16" s="69">
-        <v>1.3771867981000101</v>
-      </c>
-      <c r="M16" s="69">
-        <v>1.7106868645080799</v>
-      </c>
-      <c r="N16" s="66" t="s">
+      <c r="O16" s="59">
+        <v>1.7626712227760299</v>
+      </c>
+      <c r="P16" s="59">
+        <v>1.2204338989442101</v>
+      </c>
+      <c r="Q16" s="57">
+        <v>45.645506291878398</v>
+      </c>
+      <c r="R16" s="59">
+        <v>0.68859344211075602</v>
+      </c>
+      <c r="S16" s="59">
+        <v>1.0716785380426299</v>
+      </c>
+      <c r="T16" s="59">
+        <v>2.4440667414997699</v>
+      </c>
+      <c r="U16" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O16" s="69">
-        <v>1.7626712227760299</v>
-      </c>
-      <c r="P16" s="69">
-        <v>1.2204338989442101</v>
-      </c>
-      <c r="Q16" s="67">
-        <v>45.645506291878398</v>
-      </c>
-      <c r="R16" s="69">
-        <v>0.68859344211075602</v>
-      </c>
-      <c r="S16" s="69">
-        <v>1.0716785380426299</v>
-      </c>
-      <c r="T16" s="69">
-        <v>2.4440667414997699</v>
-      </c>
-      <c r="U16" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V16" s="67">
+      <c r="V16" s="57">
         <v>808.04554156204495</v>
       </c>
-      <c r="W16" s="67">
+      <c r="W16" s="57">
         <v>691.90043977269102</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A17" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="66">
+      <c r="C17" s="56">
         <v>7.2820712084301437E-2</v>
       </c>
-      <c r="D17" s="67">
+      <c r="D17" s="57">
         <f t="shared" si="0"/>
         <v>45.418278126978812</v>
       </c>
-      <c r="E17" s="66">
+      <c r="E17" s="56">
         <v>9.16</v>
       </c>
-      <c r="F17" s="66">
+      <c r="F17" s="56">
         <v>9.6176299999999983</v>
       </c>
-      <c r="G17" s="67">
+      <c r="G17" s="57">
         <v>94</v>
       </c>
-      <c r="H17" s="68">
+      <c r="H17" s="58">
         <v>4.8889096485901541E-3</v>
       </c>
-      <c r="I17" s="66">
+      <c r="I17" s="56">
         <v>0.498</v>
       </c>
-      <c r="J17" s="66">
+      <c r="J17" s="56">
         <v>6.2E-2</v>
       </c>
-      <c r="K17" s="66" t="s">
+      <c r="K17" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L17" s="59">
+        <v>1.91615824372271</v>
+      </c>
+      <c r="M17" s="59">
+        <v>1.00846286779506</v>
+      </c>
+      <c r="N17" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L17" s="69">
-        <v>1.91615824372271</v>
-      </c>
-      <c r="M17" s="69">
-        <v>1.00846286779506</v>
-      </c>
-      <c r="N17" s="66" t="s">
+      <c r="O17" s="59">
+        <v>1.6508560629165301</v>
+      </c>
+      <c r="P17" s="59">
+        <v>0.876992751375542</v>
+      </c>
+      <c r="Q17" s="57">
+        <v>35.718952044786</v>
+      </c>
+      <c r="R17" s="59">
+        <v>0.45660301592788299</v>
+      </c>
+      <c r="S17" s="59">
+        <v>0.21255657969849501</v>
+      </c>
+      <c r="T17" s="59">
+        <v>2.1743751557159299</v>
+      </c>
+      <c r="U17" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O17" s="69">
-        <v>1.6508560629165301</v>
-      </c>
-      <c r="P17" s="69">
-        <v>0.876992751375542</v>
-      </c>
-      <c r="Q17" s="67">
-        <v>35.718952044786</v>
-      </c>
-      <c r="R17" s="69">
-        <v>0.45660301592788299</v>
-      </c>
-      <c r="S17" s="69">
-        <v>0.21255657969849501</v>
-      </c>
-      <c r="T17" s="69">
-        <v>2.1743751557159299</v>
-      </c>
-      <c r="U17" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V17" s="67">
+      <c r="V17" s="57">
         <v>531.39461251699697</v>
       </c>
-      <c r="W17" s="67">
+      <c r="W17" s="57">
         <v>333.44539134222299</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A18" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="66">
+      <c r="C18" s="56">
         <v>0.11799999999999999</v>
       </c>
-      <c r="D18" s="67">
+      <c r="D18" s="57">
         <f t="shared" si="0"/>
         <v>73.596599999999995</v>
       </c>
-      <c r="E18" s="66">
+      <c r="E18" s="56">
         <v>9.07</v>
       </c>
-      <c r="F18" s="66">
+      <c r="F18" s="56">
         <v>9.8334700000000002</v>
       </c>
-      <c r="G18" s="67">
+      <c r="G18" s="57">
         <v>105</v>
       </c>
-      <c r="H18" s="68">
+      <c r="H18" s="58">
         <v>6.4081038062009012E-3</v>
       </c>
-      <c r="I18" s="66">
+      <c r="I18" s="56">
         <v>0.84599999999999997</v>
       </c>
-      <c r="J18" s="66">
+      <c r="J18" s="56">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="K18" s="66" t="s">
+      <c r="K18" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L18" s="59">
+        <v>1.2967854716739451</v>
+      </c>
+      <c r="M18" s="59">
+        <v>1.6651827584696051</v>
+      </c>
+      <c r="N18" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L18" s="69">
-        <v>1.2967854716739451</v>
-      </c>
-      <c r="M18" s="69">
-        <v>1.6651827584696051</v>
-      </c>
-      <c r="N18" s="66" t="s">
+      <c r="O18" s="59">
+        <v>1.7564883769297599</v>
+      </c>
+      <c r="P18" s="59">
+        <v>1.30049682050844</v>
+      </c>
+      <c r="Q18" s="57">
+        <v>46.241081793096399</v>
+      </c>
+      <c r="R18" s="59">
+        <v>0.89393402598546601</v>
+      </c>
+      <c r="S18" s="59">
+        <v>0.58531574895362004</v>
+      </c>
+      <c r="T18" s="59">
+        <v>2.3195561528830599</v>
+      </c>
+      <c r="U18" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O18" s="69">
-        <v>1.7564883769297599</v>
-      </c>
-      <c r="P18" s="69">
-        <v>1.30049682050844</v>
-      </c>
-      <c r="Q18" s="67">
-        <v>46.241081793096399</v>
-      </c>
-      <c r="R18" s="69">
-        <v>0.89393402598546601</v>
-      </c>
-      <c r="S18" s="69">
-        <v>0.58531574895362004</v>
-      </c>
-      <c r="T18" s="69">
-        <v>2.3195561528830599</v>
-      </c>
-      <c r="U18" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V18" s="67">
+      <c r="V18" s="57">
         <v>945.25629287186507</v>
       </c>
-      <c r="W18" s="67">
+      <c r="W18" s="57">
         <v>741.47910610500401</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A19" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="C19" s="66">
+      <c r="C19" s="56">
         <v>3.0202027508653907E-2</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="57">
         <f t="shared" si="0"/>
         <v>18.837004557147441</v>
       </c>
-      <c r="E19" s="66">
+      <c r="E19" s="56">
         <v>9.15</v>
       </c>
-      <c r="F19" s="66">
+      <c r="F19" s="56">
         <v>11.452219999999999</v>
       </c>
-      <c r="G19" s="67">
+      <c r="G19" s="57">
         <v>105</v>
       </c>
-      <c r="H19" s="68">
+      <c r="H19" s="58">
         <v>1.7077055898053233E-2</v>
       </c>
-      <c r="I19" s="66">
+      <c r="I19" s="56">
         <v>0.83</v>
       </c>
-      <c r="J19" s="66">
+      <c r="J19" s="56">
         <v>0.11</v>
       </c>
-      <c r="K19" s="66" t="s">
+      <c r="K19" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L19" s="59">
+        <v>7.0245446586945999</v>
+      </c>
+      <c r="M19" s="59">
+        <v>0.97941407127864799</v>
+      </c>
+      <c r="N19" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L19" s="69">
-        <v>7.0245446586945999</v>
-      </c>
-      <c r="M19" s="69">
-        <v>0.97941407127864799</v>
-      </c>
-      <c r="N19" s="66" t="s">
+      <c r="O19" s="59">
+        <v>0.718923197854207</v>
+      </c>
+      <c r="P19" s="59">
+        <v>0.63974662113902303</v>
+      </c>
+      <c r="Q19" s="57">
+        <v>16.551068661364301</v>
+      </c>
+      <c r="R19" s="59">
+        <v>0.47030881185877998</v>
+      </c>
+      <c r="S19" s="59">
+        <v>0.271575612230602</v>
+      </c>
+      <c r="T19" s="59">
+        <v>1.28345207295728</v>
+      </c>
+      <c r="U19" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O19" s="69">
-        <v>0.718923197854207</v>
-      </c>
-      <c r="P19" s="69">
-        <v>0.63974662113902303</v>
-      </c>
-      <c r="Q19" s="67">
-        <v>16.551068661364301</v>
-      </c>
-      <c r="R19" s="69">
-        <v>0.47030881185877998</v>
-      </c>
-      <c r="S19" s="69">
-        <v>0.271575612230602</v>
-      </c>
-      <c r="T19" s="69">
-        <v>1.28345207295728</v>
-      </c>
-      <c r="U19" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V19" s="67">
+      <c r="V19" s="57">
         <v>720.28980585241402</v>
       </c>
-      <c r="W19" s="67">
+      <c r="W19" s="57">
         <v>337.69358232652797</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A20" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C20" s="66">
+      <c r="C20" s="56">
         <v>3.5944003309607307E-2</v>
       </c>
-      <c r="D20" s="67">
+      <c r="D20" s="57">
         <f t="shared" si="0"/>
         <v>22.418274864202079</v>
       </c>
-      <c r="E20" s="66">
+      <c r="E20" s="56">
         <v>9.17</v>
       </c>
-      <c r="F20" s="66">
+      <c r="F20" s="56">
         <v>6.5076599999999996</v>
       </c>
-      <c r="G20" s="67">
+      <c r="G20" s="57">
         <v>30</v>
       </c>
-      <c r="H20" s="68">
+      <c r="H20" s="58">
         <v>2.2658800618592122E-2</v>
       </c>
-      <c r="I20" s="66">
+      <c r="I20" s="56">
         <v>0.27</v>
       </c>
-      <c r="J20" s="66">
+      <c r="J20" s="56">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="K20" s="66" t="s">
+      <c r="K20" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L20" s="59">
+        <v>1.2322388177005501</v>
+      </c>
+      <c r="M20" s="59">
+        <v>0.702089555932218</v>
+      </c>
+      <c r="N20" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L20" s="69">
-        <v>1.2322388177005501</v>
-      </c>
-      <c r="M20" s="69">
-        <v>0.702089555932218</v>
-      </c>
-      <c r="N20" s="66" t="s">
+      <c r="O20" s="59">
+        <v>0.52457713332045697</v>
+      </c>
+      <c r="P20" s="59">
+        <v>0.29611941056316798</v>
+      </c>
+      <c r="Q20" s="57">
+        <v>13.220298933374901</v>
+      </c>
+      <c r="R20" s="59">
+        <v>0.12815919755703201</v>
+      </c>
+      <c r="S20" s="59">
+        <v>0.77691543569315702</v>
+      </c>
+      <c r="T20" s="59">
+        <v>0.59462687121101898</v>
+      </c>
+      <c r="U20" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O20" s="69">
-        <v>0.52457713332045697</v>
-      </c>
-      <c r="P20" s="69">
-        <v>0.29611941056316798</v>
-      </c>
-      <c r="Q20" s="67">
-        <v>13.220298933374901</v>
-      </c>
-      <c r="R20" s="69">
-        <v>0.12815919755703201</v>
-      </c>
-      <c r="S20" s="69">
-        <v>0.77691543569315702</v>
-      </c>
-      <c r="T20" s="69">
-        <v>0.59462687121101898</v>
-      </c>
-      <c r="U20" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V20" s="67">
+      <c r="V20" s="57">
         <v>488.53812615076703</v>
       </c>
-      <c r="W20" s="67">
+      <c r="W20" s="57">
         <v>249.97651740093099</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A21" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="C21" s="66">
+      <c r="C21" s="56">
         <v>3.1096924160320834E-2</v>
       </c>
-      <c r="D21" s="67">
+      <c r="D21" s="57">
         <f t="shared" si="0"/>
         <v>19.395151598792104</v>
       </c>
-      <c r="E21" s="66">
+      <c r="E21" s="56">
         <v>9.16</v>
       </c>
-      <c r="F21" s="66">
+      <c r="F21" s="56">
         <v>7.80267</v>
       </c>
-      <c r="G21" s="67">
+      <c r="G21" s="57">
         <v>38</v>
       </c>
-      <c r="H21" s="68">
+      <c r="H21" s="58">
         <v>1.0794792231033178E-2</v>
       </c>
-      <c r="I21" s="66">
+      <c r="I21" s="56">
         <v>0.29599999999999999</v>
       </c>
-      <c r="J21" s="66">
+      <c r="J21" s="56">
         <v>5.5E-2</v>
       </c>
-      <c r="K21" s="66" t="s">
+      <c r="K21" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L21" s="59">
+        <v>1.1643336675989699</v>
+      </c>
+      <c r="M21" s="59">
+        <v>0.63279001194044404</v>
+      </c>
+      <c r="N21" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L21" s="69">
-        <v>1.1643336675989699</v>
-      </c>
-      <c r="M21" s="69">
-        <v>0.63279001194044404</v>
-      </c>
-      <c r="N21" s="66" t="s">
+      <c r="O21" s="59">
+        <v>0.46634706396213099</v>
+      </c>
+      <c r="P21" s="59">
+        <v>0.37507190657484901</v>
+      </c>
+      <c r="Q21" s="57">
+        <v>10.360115031825201</v>
+      </c>
+      <c r="R21" s="59">
+        <v>0.16874401122045901</v>
+      </c>
+      <c r="S21" s="59">
+        <v>0.78772770621289701</v>
+      </c>
+      <c r="T21" s="59">
+        <v>0.454074777269866</v>
+      </c>
+      <c r="U21" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O21" s="69">
-        <v>0.46634706396213099</v>
-      </c>
-      <c r="P21" s="69">
-        <v>0.37507190657484901</v>
-      </c>
-      <c r="Q21" s="67">
-        <v>10.360115031825201</v>
-      </c>
-      <c r="R21" s="69">
-        <v>0.16874401122045901</v>
-      </c>
-      <c r="S21" s="69">
-        <v>0.78772770621289701</v>
-      </c>
-      <c r="T21" s="69">
-        <v>0.454074777269866</v>
-      </c>
-      <c r="U21" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V21" s="67">
+      <c r="V21" s="57">
         <v>484.032965517913</v>
       </c>
-      <c r="W21" s="67">
+      <c r="W21" s="57">
         <v>257.88992371906602</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A22" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" s="66">
+      <c r="C22" s="56">
         <v>7.9405319091762502E-2</v>
       </c>
-      <c r="D22" s="67">
+      <c r="D22" s="57">
         <f t="shared" si="0"/>
         <v>49.525097517532274</v>
       </c>
-      <c r="E22" s="66">
+      <c r="E22" s="56">
         <v>9.1</v>
       </c>
-      <c r="F22" s="66">
+      <c r="F22" s="56">
         <v>11.27563</v>
       </c>
-      <c r="G22" s="67">
+      <c r="G22" s="57">
         <v>119</v>
       </c>
-      <c r="H22" s="68">
+      <c r="H22" s="58">
         <v>1.0354892780764112E-2</v>
       </c>
-      <c r="I22" s="66">
+      <c r="I22" s="56">
         <v>0.80900000000000005</v>
       </c>
-      <c r="J22" s="66">
+      <c r="J22" s="56">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="K22" s="66" t="s">
+      <c r="K22" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L22" s="59">
+        <v>2.72764747230935</v>
+      </c>
+      <c r="M22" s="59">
+        <v>1.45961334900535</v>
+      </c>
+      <c r="N22" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L22" s="69">
-        <v>2.72764747230935</v>
-      </c>
-      <c r="M22" s="69">
-        <v>1.45961334900535</v>
-      </c>
-      <c r="N22" s="66" t="s">
+      <c r="O22" s="59">
+        <v>1.4407694685627599</v>
+      </c>
+      <c r="P22" s="59">
+        <v>1.31435862140282</v>
+      </c>
+      <c r="Q22" s="57">
+        <v>37.566001980104502</v>
+      </c>
+      <c r="R22" s="59">
+        <v>0.65482382507480497</v>
+      </c>
+      <c r="S22" s="59">
+        <v>0.92491901667315302</v>
+      </c>
+      <c r="T22" s="59">
+        <v>2.26440281809306</v>
+      </c>
+      <c r="U22" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O22" s="69">
-        <v>1.4407694685627599</v>
-      </c>
-      <c r="P22" s="69">
-        <v>1.31435862140282</v>
-      </c>
-      <c r="Q22" s="67">
-        <v>37.566001980104502</v>
-      </c>
-      <c r="R22" s="69">
-        <v>0.65482382507480497</v>
-      </c>
-      <c r="S22" s="69">
-        <v>0.92491901667315302</v>
-      </c>
-      <c r="T22" s="69">
-        <v>2.26440281809306</v>
-      </c>
-      <c r="U22" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V22" s="67">
+      <c r="V22" s="57">
         <v>747.09904434894099</v>
       </c>
-      <c r="W22" s="67">
+      <c r="W22" s="57">
         <v>484.71645920348499</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A23" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23" s="66">
+      <c r="C23" s="56">
         <v>9.398160324751717E-2</v>
       </c>
-      <c r="D23" s="67">
+      <c r="D23" s="57">
         <f t="shared" si="0"/>
         <v>58.616325945476461</v>
       </c>
-      <c r="E23" s="66">
+      <c r="E23" s="56">
         <v>9.18</v>
       </c>
-      <c r="F23" s="66">
+      <c r="F23" s="56">
         <v>7.80267</v>
       </c>
-      <c r="G23" s="67">
+      <c r="G23" s="57">
         <v>98</v>
       </c>
-      <c r="H23" s="68">
+      <c r="H23" s="58">
         <v>3.4287377107106464E-3</v>
       </c>
-      <c r="I23" s="66">
+      <c r="I23" s="56">
         <v>0.53500000000000003</v>
       </c>
-      <c r="J23" s="66">
+      <c r="J23" s="56">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="K23" s="66" t="s">
+      <c r="K23" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L23" s="59">
+        <v>1.3720608964846499</v>
+      </c>
+      <c r="M23" s="59">
+        <v>1.1958110872549399</v>
+      </c>
+      <c r="N23" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L23" s="69">
-        <v>1.3720608964846499</v>
-      </c>
-      <c r="M23" s="69">
-        <v>1.1958110872549399</v>
-      </c>
-      <c r="N23" s="66" t="s">
+      <c r="O23" s="59">
+        <v>1.2179411085780001</v>
+      </c>
+      <c r="P23" s="59">
+        <v>0.64414145630695796</v>
+      </c>
+      <c r="Q23" s="57">
+        <v>39.430151356215198</v>
+      </c>
+      <c r="R23" s="59">
+        <v>0.52084568302767098</v>
+      </c>
+      <c r="S23" s="59">
+        <v>1.6297174169008599</v>
+      </c>
+      <c r="T23" s="59">
+        <v>1.4803398730307999</v>
+      </c>
+      <c r="U23" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O23" s="69">
-        <v>1.2179411085780001</v>
-      </c>
-      <c r="P23" s="69">
-        <v>0.64414145630695796</v>
-      </c>
-      <c r="Q23" s="67">
-        <v>39.430151356215198</v>
-      </c>
-      <c r="R23" s="69">
-        <v>0.52084568302767098</v>
-      </c>
-      <c r="S23" s="69">
-        <v>1.6297174169008599</v>
-      </c>
-      <c r="T23" s="69">
-        <v>1.4803398730307999</v>
-      </c>
-      <c r="U23" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V23" s="67">
+      <c r="V23" s="57">
         <v>557.10493581988896</v>
       </c>
-      <c r="W23" s="67">
+      <c r="W23" s="57">
         <v>400.91998923722298</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A24" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C24" s="66">
+      <c r="C24" s="56">
         <v>0.39148074291205415</v>
       </c>
-      <c r="D24" s="67">
+      <c r="D24" s="57">
         <f t="shared" si="0"/>
         <v>244.16653935424819</v>
       </c>
-      <c r="E24" s="66">
+      <c r="E24" s="56">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F24" s="66">
+      <c r="F24" s="56">
         <v>22.214490000000001</v>
       </c>
-      <c r="G24" s="67">
+      <c r="G24" s="57">
         <v>184</v>
       </c>
-      <c r="H24" s="68">
+      <c r="H24" s="58">
         <v>8.8635224370739608E-3</v>
       </c>
-      <c r="I24" s="66">
+      <c r="I24" s="56">
         <v>3.11</v>
       </c>
-      <c r="J24" s="66">
+      <c r="J24" s="56">
         <v>0.32300000000000001</v>
       </c>
-      <c r="K24" s="66" t="s">
+      <c r="K24" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L24" s="59">
+        <v>1.5426911156721901</v>
+      </c>
+      <c r="M24" s="59">
+        <v>3.5399806235861901</v>
+      </c>
+      <c r="N24" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L24" s="69">
-        <v>1.5426911156721901</v>
-      </c>
-      <c r="M24" s="69">
-        <v>3.5399806235861901</v>
-      </c>
-      <c r="N24" s="66" t="s">
+      <c r="O24" s="59">
+        <v>2.49680550904207</v>
+      </c>
+      <c r="P24" s="59">
+        <v>3.4772505621278902</v>
+      </c>
+      <c r="Q24" s="57">
+        <v>51.711905605203903</v>
+      </c>
+      <c r="R24" s="59">
+        <v>1.77037757925062</v>
+      </c>
+      <c r="S24" s="59">
+        <v>0.66679575104565703</v>
+      </c>
+      <c r="T24" s="59">
+        <v>4.6559536175050402</v>
+      </c>
+      <c r="U24" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O24" s="69">
-        <v>2.49680550904207</v>
-      </c>
-      <c r="P24" s="69">
-        <v>3.4772505621278902</v>
-      </c>
-      <c r="Q24" s="67">
-        <v>51.711905605203903</v>
-      </c>
-      <c r="R24" s="69">
-        <v>1.77037757925062</v>
-      </c>
-      <c r="S24" s="69">
-        <v>0.66679575104565703</v>
-      </c>
-      <c r="T24" s="69">
-        <v>4.6559536175050402</v>
-      </c>
-      <c r="U24" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V24" s="67">
+      <c r="V24" s="57">
         <v>1714.0693617813399</v>
       </c>
-      <c r="W24" s="67">
+      <c r="W24" s="57">
         <v>1553.85018188402</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="20.100000000000001" customHeight="1">
+    <row r="25" spans="1:23" ht="20.149999999999999" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="66">
+        <v>162</v>
+      </c>
+      <c r="C25" s="56">
         <v>9.5557081789423903E-2</v>
       </c>
-      <c r="D25" s="67">
+      <c r="D25" s="57">
         <f t="shared" si="0"/>
         <v>59.59895191206369</v>
       </c>
-      <c r="E25" s="66">
+      <c r="E25" s="56">
         <v>9.06</v>
       </c>
-      <c r="F25" s="66">
+      <c r="F25" s="56">
         <v>21.82206</v>
       </c>
-      <c r="G25" s="67">
+      <c r="G25" s="57">
         <v>266</v>
       </c>
-      <c r="H25" s="68">
+      <c r="H25" s="58">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I25" s="66">
+      <c r="I25" s="56">
         <v>1.81</v>
       </c>
-      <c r="J25" s="66">
+      <c r="J25" s="56">
         <v>0.221</v>
       </c>
-      <c r="K25" s="66" t="s">
+      <c r="K25" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="L25" s="59">
+        <v>6.7677874291210802</v>
+      </c>
+      <c r="M25" s="59">
+        <v>2.3666928051530398</v>
+      </c>
+      <c r="N25" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="L25" s="69">
-        <v>6.7677874291210802</v>
-      </c>
-      <c r="M25" s="69">
-        <v>2.3666928051530398</v>
-      </c>
-      <c r="N25" s="66" t="s">
+      <c r="O25" s="59">
+        <v>1.70289293591274</v>
+      </c>
+      <c r="P25" s="59">
+        <v>2.4722438786933201</v>
+      </c>
+      <c r="Q25" s="57">
+        <v>84.103989326398704</v>
+      </c>
+      <c r="R25" s="59">
+        <v>1.27677870710454</v>
+      </c>
+      <c r="S25" s="59">
+        <v>1.3369819851325699</v>
+      </c>
+      <c r="T25" s="59">
+        <v>3.5293196856631899</v>
+      </c>
+      <c r="U25" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="O25" s="69">
-        <v>1.70289293591274</v>
-      </c>
-      <c r="P25" s="69">
-        <v>2.4722438786933201</v>
-      </c>
-      <c r="Q25" s="67">
-        <v>84.103989326398704</v>
-      </c>
-      <c r="R25" s="69">
-        <v>1.27677870710454</v>
-      </c>
-      <c r="S25" s="69">
-        <v>1.3369819851325699</v>
-      </c>
-      <c r="T25" s="69">
-        <v>3.5293196856631899</v>
-      </c>
-      <c r="U25" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="V25" s="67">
+      <c r="V25" s="57">
         <v>2778.00626260541</v>
       </c>
-      <c r="W25" s="67">
+      <c r="W25" s="57">
         <v>1034.2822572547</v>
       </c>
     </row>
     <row r="26" spans="1:23">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="70"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="70"/>
-      <c r="O26" s="70"/>
-      <c r="P26" s="70"/>
-      <c r="Q26" s="70"/>
-      <c r="R26" s="70"/>
-      <c r="S26" s="70"/>
-      <c r="T26" s="70"/>
-      <c r="U26" s="70"/>
-      <c r="V26" s="70"/>
-      <c r="W26" s="70"/>
-    </row>
-    <row r="27" spans="1:23" ht="6.95" customHeight="1"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="60"/>
+      <c r="Q26" s="60"/>
+      <c r="R26" s="60"/>
+      <c r="S26" s="60"/>
+      <c r="T26" s="60"/>
+      <c r="U26" s="60"/>
+      <c r="V26" s="60"/>
+      <c r="W26" s="60"/>
+    </row>
+    <row r="27" spans="1:23" ht="7" customHeight="1"/>
     <row r="28" spans="1:23" ht="18" customHeight="1">
-      <c r="A28" s="71" t="s">
-        <v>165</v>
+      <c r="A28" s="61" t="s">
+        <v>163</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="37"/>
@@ -4480,11 +4492,11 @@
       <c r="V28" s="37"/>
       <c r="W28" s="37"/>
     </row>
-    <row r="29" spans="1:23" ht="18.95" customHeight="1">
-      <c r="A29" s="72" t="s">
-        <v>166</v>
-      </c>
-      <c r="B29" s="73"/>
+    <row r="29" spans="1:23" ht="19" customHeight="1">
+      <c r="A29" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="63"/>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
       <c r="E29" s="3"/>
@@ -4507,11 +4519,11 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="1:23" ht="18.95" customHeight="1">
+    <row r="30" spans="1:23" ht="19" customHeight="1">
       <c r="A30" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="B30" s="73"/>
+        <v>165</v>
+      </c>
+      <c r="B30" s="63"/>
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
@@ -4534,7 +4546,7 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:23" s="22" customFormat="1" ht="18.95" customHeight="1">
+    <row r="31" spans="1:23" s="22" customFormat="1" ht="19" customHeight="1">
       <c r="A31" s="27" t="str">
         <f ca="1">IF(OFFSET(A31,-1,,,)="Notes: ","1. Analysis conducted between sample arrival date and reporting date.",
 IF(NOT(ISERROR(VALUE(LEFT(OFFSET(A31,-1,,,),2)))),VALUE(LEFT(OFFSET(A31,-1,,,),2))+1&amp;". Analysis conducted between sample arrival date and reporting date.",
@@ -4554,7 +4566,7 @@
       <c r="C31" s="36"/>
       <c r="D31" s="36"/>
     </row>
-    <row r="32" spans="1:23" s="22" customFormat="1" ht="18.95" customHeight="1">
+    <row r="32" spans="1:23" s="22" customFormat="1" ht="19" customHeight="1">
       <c r="A32" s="27" t="str">
         <f ca="1">IF(OFFSET(A32,-1,,,)="Notes: ","1. ** NATA accreditation does not cover the performance of this service.",
 IF(NOT(ISERROR(VALUE(LEFT(OFFSET(A32,-1,,,),2)))),VALUE(LEFT(OFFSET(A32,-1,,,),2))+1&amp;". ** NATA accreditation does not cover the performance of this service.",
@@ -4574,7 +4586,7 @@
       <c r="C32" s="36"/>
       <c r="D32" s="36"/>
     </row>
-    <row r="33" spans="1:23" s="22" customFormat="1" ht="18.95" customHeight="1">
+    <row r="33" spans="1:23" s="22" customFormat="1" ht="19" customHeight="1">
       <c r="A33" s="27" t="str">
         <f ca="1">IF(OFFSET(A33,-1,,,)="Notes: ","1. .. Denotes not requested.",
 IF(NOT(ISERROR(VALUE(LEFT(OFFSET(A33,-1,,,),2)))),VALUE(LEFT(OFFSET(A33,-1,,,),2))+1&amp;". .. Denotes not requested.",
@@ -4594,7 +4606,7 @@
       <c r="C33" s="36"/>
       <c r="D33" s="36"/>
     </row>
-    <row r="34" spans="1:23" s="22" customFormat="1" ht="18.95" customHeight="1">
+    <row r="34" spans="1:23" s="22" customFormat="1" ht="19" customHeight="1">
       <c r="A34" s="27" t="str">
         <f ca="1">IF(OFFSET(A34,-1,,,)="Notes: ","1. This report is not to be reproduced except in full.",
 IF(NOT(ISERROR(VALUE(LEFT(OFFSET(A34,-1,,,),2)))),VALUE(LEFT(OFFSET(A34,-1,,,),2))+1&amp;". This report is not to be reproduced except in full.",
@@ -4614,7 +4626,7 @@
       <c r="C34" s="36"/>
       <c r="D34" s="36"/>
     </row>
-    <row r="35" spans="1:23" ht="18.95" customHeight="1">
+    <row r="35" spans="1:23" ht="19" customHeight="1">
       <c r="A35" s="27" t="str">
         <f ca="1">IF(OFFSET(A35,-1,,,)="Notes: ","1. All services undertaken by EAL are covered by the EAL Laboratory Services Terms and Conditions (refer scu.edu.au/eal or on request).",
 IF(NOT(ISERROR(VALUE(LEFT(OFFSET(A35,-1,,,),2)))),VALUE(LEFT(OFFSET(A35,-1,,,),2))+1&amp;". All services undertaken by EAL are covered by the EAL Laboratory Services Terms and Conditions (refer scu.edu.au/eal or on request).",
@@ -4653,9 +4665,9 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
     </row>
-    <row r="36" spans="1:23" ht="18.95" customHeight="1">
+    <row r="36" spans="1:23" ht="19" customHeight="1">
       <c r="A36" s="27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="37"/>
@@ -4681,15 +4693,15 @@
       <c r="W36" s="3"/>
     </row>
     <row r="37" spans="1:23" hidden="1">
-      <c r="A37" s="74" t="s">
-        <v>169</v>
+      <c r="A37" s="64" t="s">
+        <v>167</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
@@ -4717,7 +4729,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.51" right="0.51" top="0.51" bottom="1.3737007874015748" header="0.39000000000000007" footer="0.39000000000000007"/>
-  <pageSetup paperSize="9" scale="62" fitToWidth="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="63" fitToWidth="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;12PAGE &amp;P OF &amp;N</oddHeader>
     <oddFooter>&amp;C&amp;12&amp;K008000Environmental Analysis Laboratory, Southern Cross University, 

</xml_diff>